<commit_message>
Changes on the ingestion and removed a file from the doc
</commit_message>
<xml_diff>
--- a/docs/Report-Initial-Analysis.xlsx
+++ b/docs/Report-Initial-Analysis.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\leand\OneDrive\Área de Trabalho\AISCB_FraudDetection\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD349A27-423F-46B2-96FB-40A9853051E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CE12C53-B600-43C3-8575-D6B6BFD75F03}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{1E9FE23F-168F-4DDA-AB37-4186E608AA4A}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{1E9FE23F-168F-4DDA-AB37-4186E608AA4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Jissy</t>
   </si>
@@ -96,9 +96,6 @@
   </si>
   <si>
     <t>Sushma</t>
-  </si>
-  <si>
-    <t>This is an addition so Git can check I've made a change in my file</t>
   </si>
 </sst>
 </file>
@@ -480,30 +477,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A9438122-7B02-4BF4-A267-A7655FAF6FEC}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" customWidth="1"/>
-    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.7265625" customWidth="1"/>
+    <col min="2" max="2" width="30.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="58" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>18</v>
       </c>
@@ -511,7 +505,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -519,7 +513,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -527,7 +521,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>3</v>
       </c>
@@ -535,7 +529,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>4</v>
       </c>
@@ -543,7 +537,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>5</v>
       </c>
@@ -551,7 +545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>6</v>
       </c>
@@ -559,7 +553,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>7</v>
       </c>
@@ -567,7 +561,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>19</v>
       </c>

</xml_diff>